<commit_message>
organize normalize to survey
</commit_message>
<xml_diff>
--- a/test/fixture/advanced_notes.xlsx
+++ b/test/fixture/advanced_notes.xlsx
@@ -1,14 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="survey" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="settings" sheetId="2" r:id="rId4"/>
-    <sheet state="visible" name="choices" sheetId="3" r:id="rId5"/>
+    <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="settings" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="choices" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
@@ -51,7 +55,7 @@
     <t>required</t>
   </si>
   <si>
-    <t xml:space="preserve">note </t>
+    <t>note </t>
   </si>
   <si>
     <t>note1</t>
@@ -67,7 +71,7 @@
     <t>note2</t>
   </si>
   <si>
-    <t xml:space="preserve">Subsequent notes are visually fused together to get around the limitation of only one image (and video and audio) per note. </t>
+    <t>Subsequent notes are visually fused together to get around the limitation of only one image (and video and audio) per note. </t>
   </si>
   <si>
     <t>tiger.png</t>
@@ -213,183 +217,261 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+  </numFmts>
+  <fonts count="9">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Ubuntu"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
-    <font/>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Ubuntu"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Ubuntu"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="3">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom style="thin"/>
+      <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <top style="thin"/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/worksheetdrawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="7.0"/>
-    <col customWidth="1" min="2" max="2" width="7.14"/>
-    <col customWidth="1" min="3" max="3" width="47.57"/>
-    <col customWidth="1" min="4" max="4" width="15.71"/>
-    <col customWidth="1" min="5" max="5" width="13.29"/>
-    <col customWidth="1" min="6" max="6" width="6.71"/>
-    <col customWidth="1" min="7" max="7" width="17.57"/>
-    <col customWidth="1" min="8" max="8" width="10.86"/>
-    <col customWidth="1" min="9" max="9" width="11.29"/>
-    <col customWidth="1" min="10" max="10" width="13.14"/>
-    <col customWidth="1" min="11" max="11" width="14.86"/>
-    <col customWidth="1" min="12" max="12" width="10.57"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.13775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.7142857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.2908163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.71428571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.5765306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.8622448979592"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.2959183673469"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.1377551020408"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="14.8571428571429"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.5765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="14.4285714285714"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" ht="15.0" customHeight="1">
-      <c r="A2" s="2" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="3"/>
@@ -402,7 +484,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
@@ -415,16 +497,16 @@
       <c r="D3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
@@ -437,279 +519,311 @@
       <c r="D4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="6" t="s">
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-    </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="6" t="s">
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="6" t="s">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="6" t="s">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="27.71"/>
-    <col customWidth="1" min="2" max="2" width="21.29"/>
-    <col customWidth="1" min="3" max="3" width="22.57"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.7091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.2908163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.5714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="14.4285714285714"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="7" t="s">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="9" t="s">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" min="1" max="3" width="16.86"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="16.8673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="14.4285714285714"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="11" t="s">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="4" t="s">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="4" t="s">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="4" t="s">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" ht="15.0" customHeight="1">
-      <c r="A5" s="4" t="s">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="4" t="s">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="4" t="s">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="4" t="s">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" ht="15.0" customHeight="1">
-      <c r="A10" s="4" t="s">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" ht="15.0" customHeight="1">
-      <c r="A11" s="4" t="s">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="4" t="s">
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" ht="15.0" customHeight="1">
-      <c r="A13" s="4" t="s">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="4" t="s">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="4" t="s">
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="11" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>